<commit_message>
A lot of additions and changes
</commit_message>
<xml_diff>
--- a/Gantt Chart for Capstone.xlsx
+++ b/Gantt Chart for Capstone.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burni\Google Drive\9SSenior 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\CSCapstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12213"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Week 1</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Research / Proof of Concept (Base Station App)</t>
   </si>
   <si>
-    <t>Survivor Visualization</t>
-  </si>
-  <si>
     <t>Google Maps Implementation</t>
   </si>
   <si>
@@ -89,18 +86,62 @@
     <t xml:space="preserve">  Device Communication</t>
   </si>
   <si>
-    <t>Finalize design and ensure compatibilty between apps</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Database Creation</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Survivor Visualization (3D)</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Companion application able to visualize data from base station</t>
+  </si>
+  <si>
+    <t>2D Visualization utilizing some surface map</t>
+  </si>
+  <si>
+    <t>3D Visualization able to demonstrate depth</t>
+  </si>
+  <si>
+    <t>Optionals</t>
+  </si>
+  <si>
+    <t>Base station application able to set rescue grid and receive data from drones</t>
+  </si>
+  <si>
+    <t>Augmented Reality view</t>
+  </si>
+  <si>
+    <t>Data analysis settings for different material types</t>
+  </si>
+  <si>
+    <t>Optional Development</t>
+  </si>
+  <si>
+    <t>Base Station</t>
+  </si>
+  <si>
+    <t>AR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,12 +155,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -139,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,34 +193,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,23 +542,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.5859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.64453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.87890625" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1171875" style="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="13" width="9.1171875" style="1"/>
+    <col min="14" max="14" width="61.9375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,81 +603,133 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E4" s="3" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="8"/>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J7" s="4" t="s">
+      <c r="K9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N10" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N15" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="N16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.5">
+      <c r="N17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.5">
+      <c r="N18" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="K8:L8"/>
+  <mergeCells count="7">
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J8:M8"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>